<commit_message>
improved after peer review
</commit_message>
<xml_diff>
--- a/cloud-architecture/oracle-apps-hyperion-siebel-gbu/gbu/retail-gbu/rgbu-discovery-questionnaire/files/rgbu-discovery-questionnaire.xlsx
+++ b/cloud-architecture/oracle-apps-hyperion-siebel-gbu/gbu/retail-gbu/rgbu-discovery-questionnaire/files/rgbu-discovery-questionnaire.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933BB3F4-D252-4231-891F-0AA6ECED488B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2EF5A2-5B32-4A9B-8D68-D90C54973CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
-    <sheet name="PrjInfo" sheetId="24" r:id="rId2"/>
-    <sheet name="HW SW" sheetId="6" r:id="rId3"/>
+    <sheet name="Project Information" sheetId="24" r:id="rId2"/>
+    <sheet name="Current HW &amp; SW Inventory" sheetId="6" r:id="rId3"/>
     <sheet name="MOM" sheetId="11" r:id="rId4"/>
     <sheet name="RTG" sheetId="15" r:id="rId5"/>
     <sheet name="P&amp;O" sheetId="17" r:id="rId6"/>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="214">
   <si>
     <t xml:space="preserve">Customer </t>
   </si>
@@ -290,9 +290,6 @@
     <t>Microsoft, Google ... Yes/No</t>
   </si>
   <si>
-    <t xml:space="preserve">Is an OCI UC contract already signed and in place? </t>
-  </si>
-  <si>
     <t>Is the customer already consuming OCI?</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
   </si>
   <si>
     <t>backup, CIS compliance, ...</t>
-  </si>
-  <si>
-    <t>Did the customer subscribe to C@C or other Engineered Systems ?</t>
   </si>
   <si>
     <t>Environment</t>
@@ -1798,14 +1792,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1859,9 +1847,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1873,15 +1858,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -1909,6 +1885,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -6267,124 +6255,111 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:C18"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="80.5703125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" style="31" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="3.85546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="80.5703125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-    </row>
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6396,439 +6371,369 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEB2732-A08B-4C96-921E-66403E60296D}">
   <dimension ref="B1:C71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="21"/>
-    <col min="2" max="2" width="72.42578125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" style="26" customWidth="1"/>
-    <col min="4" max="16384" width="7.28515625" style="21"/>
+    <col min="1" max="1" width="7.28515625" style="19"/>
+    <col min="2" max="2" width="72.42578125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="7.28515625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B1" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="33"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="36"/>
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="C6" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="C8" s="20"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="C10" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="C11"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="C13" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="C14"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="C16" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
+      <c r="C17"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="C19" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="C20"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="C22" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="C24"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="C23"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
+      <c r="C26" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="C24"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
+      <c r="C27"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C26" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
+      <c r="C29" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C27"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
+      <c r="C32"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="C31"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="24" t="s">
+      <c r="C34" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="24" t="s">
+      <c r="C35"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="C35"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="24" t="s">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C36"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
+      <c r="C38"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="C37"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="24" t="s">
+      <c r="C40" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C38"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="24" t="s">
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="C40" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="24" t="s">
+      <c r="C42"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C41"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="C43"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="C42"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="C44"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C43"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="C46" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="C44"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="22"/>
-      <c r="C45" s="23"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
+      <c r="C47"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="C46" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="24" t="s">
+      <c r="C49" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="C47"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="22"/>
-      <c r="C48" s="23"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="24" t="s">
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C49" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="24" t="s">
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="C50"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="24" t="s">
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C51"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
+      <c r="C53"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="C52"/>
-    </row>
-    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="24" t="s">
+      <c r="C55" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C53"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="24" t="s">
+      <c r="C56"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C55" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="24" t="s">
+      <c r="C58" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B59" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="C56"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="22"/>
-      <c r="C57" s="23"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="24" t="s">
+      <c r="C59"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="C58" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B59" s="24" t="s">
+      <c r="C61" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C59"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="22"/>
-      <c r="C60" s="23"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="24" t="s">
+      <c r="C62"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C61" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="24" t="s">
+      <c r="C64" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B65" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="22"/>
-      <c r="C63" s="23"/>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="24" t="s">
+      <c r="C65"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="C64" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B65" s="24" t="s">
+      <c r="C67" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C65"/>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="22"/>
-      <c r="C66" s="23"/>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="24" t="s">
+      <c r="C68"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C67" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B68" s="24" t="s">
+      <c r="C70" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B71" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="C68"/>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="22"/>
-      <c r="C69" s="23"/>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B71" s="24" t="s">
-        <v>214</v>
       </c>
       <c r="C71"/>
     </row>
@@ -6869,481 +6774,483 @@
   </sheetPr>
   <dimension ref="B2:U38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="56.42578125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" style="21" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="21" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="37.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" style="21" customWidth="1"/>
-    <col min="15" max="15" width="27.5703125" style="21" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" style="21" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" style="21" customWidth="1"/>
-    <col min="19" max="19" width="23" style="21" customWidth="1"/>
-    <col min="20" max="20" width="29" style="21" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.7109375" style="21" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="56.42578125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" style="19" customWidth="1"/>
+    <col min="12" max="12" width="37.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" style="19" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" style="19" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" style="19" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" style="19" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" style="19" customWidth="1"/>
+    <col min="19" max="19" width="23" style="19" customWidth="1"/>
+    <col min="20" max="20" width="29" style="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.7109375" style="19" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+    </row>
+    <row r="6" spans="2:21" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-    </row>
-    <row r="6" spans="2:21" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="J6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="K6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="L6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="M6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="N6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="O6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="P6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="Q6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="R6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="S6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="T6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="U6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="T6" s="13" t="s">
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14" t="s">
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="K7" s="12">
+        <v>24</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="M7" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="14">
-        <v>1</v>
-      </c>
-      <c r="H7" s="14">
-        <v>4</v>
-      </c>
-      <c r="I7" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="J7" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="K7" s="14">
-        <v>24</v>
-      </c>
-      <c r="L7" s="14">
-        <v>0.38</v>
-      </c>
-      <c r="M7" s="14">
-        <v>0.65</v>
-      </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14" t="s">
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="11"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="11"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="16"/>
-      <c r="C33" s="10"/>
-    </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7364,217 +7271,217 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="33"/>
-    <col min="2" max="2" width="129.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="33"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="129.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="2:3" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+    </row>
+    <row r="5" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+    </row>
+    <row r="6" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="2:3" s="34" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-    </row>
-    <row r="5" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>72</v>
       </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
       <c r="C11"/>
     </row>
-    <row r="12" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B12"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-    </row>
-    <row r="14" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16"/>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18"/>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20"/>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24"/>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28"/>
     </row>
     <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29"/>
     </row>
     <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30"/>
     </row>
     <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31"/>
     </row>
     <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32"/>
     </row>
     <row r="33" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33"/>
     </row>
     <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34"/>
     </row>
     <row r="35" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35"/>
     </row>
     <row r="36" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36"/>
     </row>
     <row r="37" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C37"/>
     </row>
@@ -7605,160 +7512,160 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="33"/>
-    <col min="2" max="2" width="129.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="33"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="129.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="2:3" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+    </row>
+    <row r="5" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="2:3" s="34" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-    </row>
-    <row r="5" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>103</v>
       </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>104</v>
       </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C11"/>
+    </row>
+    <row r="12" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
       <c r="C12"/>
     </row>
-    <row r="13" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>71</v>
+        <v>105</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C18"/>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C20"/>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C24"/>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28"/>
     </row>
@@ -7793,223 +7700,223 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="33"/>
-    <col min="2" max="2" width="129.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="33"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="129.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="2:3" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+    </row>
+    <row r="5" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="2:3" s="34" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-    </row>
-    <row r="5" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
       <c r="C11"/>
     </row>
-    <row r="12" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B12"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-    </row>
-    <row r="14" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>71</v>
+        <v>122</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16"/>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18"/>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C20"/>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C24"/>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28"/>
     </row>
     <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29"/>
     </row>
     <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30"/>
     </row>
     <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31"/>
     </row>
     <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32"/>
     </row>
     <row r="33" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C33"/>
     </row>
     <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34"/>
     </row>
     <row r="35" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C35"/>
     </row>
     <row r="36" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C36"/>
     </row>
     <row r="37" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C37"/>
     </row>
     <row r="38" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C38"/>
     </row>
@@ -8040,180 +7947,180 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="33"/>
-    <col min="2" max="2" width="129.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="33"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="129.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="2:3" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+    </row>
+    <row r="5" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="2:3" s="34" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-    </row>
-    <row r="5" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>135</v>
-      </c>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>137</v>
       </c>
       <c r="C10"/>
     </row>
     <row r="11" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>71</v>
+        <v>136</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16"/>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C18"/>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C20"/>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C24"/>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28"/>
     </row>
     <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29"/>
     </row>
     <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C30"/>
     </row>
@@ -8222,86 +8129,86 @@
       <c r="C31"/>
     </row>
     <row r="33" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>71</v>
+        <v>147</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C35"/>
     </row>
     <row r="36" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C36"/>
     </row>
     <row r="37" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C37"/>
     </row>
     <row r="38" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38"/>
     </row>
     <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C39"/>
     </row>
     <row r="40" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C40"/>
     </row>
     <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C41"/>
     </row>
     <row r="42" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C42"/>
     </row>
     <row r="43" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C43"/>
     </row>
     <row r="44" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C44"/>
     </row>
     <row r="45" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C45"/>
     </row>
     <row r="46" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C46"/>
     </row>
@@ -8337,193 +8244,193 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="33"/>
-    <col min="2" max="2" width="129.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="33" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="33"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="129.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="2:3" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+    </row>
+    <row r="5" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="2:3" s="34" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-    </row>
-    <row r="5" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>72</v>
       </c>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
       <c r="C10"/>
     </row>
-    <row r="11" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11"/>
     </row>
-    <row r="12" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B12"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-    </row>
-    <row r="14" spans="2:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="2:3" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>71</v>
+        <v>155</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C16"/>
     </row>
     <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C17"/>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18"/>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C19"/>
     </row>
     <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C20"/>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21"/>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C22"/>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C23"/>
     </row>
     <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C24"/>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C25"/>
     </row>
     <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C26"/>
     </row>
     <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27"/>
     </row>
     <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28"/>
     </row>
     <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29"/>
     </row>
     <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C30"/>
     </row>
     <row r="31" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C31"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C32" s="18"/>
+      <c r="B32" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>